<commit_message>
working on project 5b
</commit_message>
<xml_diff>
--- a/school/spring-2017/algorithms/project-5/MappingNodes.xlsx
+++ b/school/spring-2017/algorithms/project-5/MappingNodes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="7">
   <si>
     <t>OXXXXXXXXX</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>graph map</t>
+  </si>
+  <si>
+    <t>Count:</t>
   </si>
 </sst>
 </file>
@@ -400,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y26"/>
+  <dimension ref="A1:Y46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="S47" sqref="S47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,6 +919,146 @@
         <v>31</v>
       </c>
     </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="P30">
+        <v>1</v>
+      </c>
+      <c r="S30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="P31">
+        <v>2</v>
+      </c>
+      <c r="S31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="P32">
+        <v>3</v>
+      </c>
+      <c r="S32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="P33">
+        <v>4</v>
+      </c>
+      <c r="S33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="P34">
+        <v>5</v>
+      </c>
+      <c r="S34">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="P35">
+        <v>6</v>
+      </c>
+      <c r="S35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="P36">
+        <v>7</v>
+      </c>
+      <c r="S36">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="P37">
+        <v>12</v>
+      </c>
+      <c r="S37">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="P38">
+        <v>16</v>
+      </c>
+      <c r="S38">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="P39">
+        <v>21</v>
+      </c>
+      <c r="S39">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="P40">
+        <v>27</v>
+      </c>
+      <c r="S40">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="P41">
+        <v>28</v>
+      </c>
+      <c r="S41">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="P42">
+        <v>29</v>
+      </c>
+      <c r="S42">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="P43">
+        <v>30</v>
+      </c>
+      <c r="S43">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="P44">
+        <v>31</v>
+      </c>
+      <c r="S44">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N46" t="s">
+        <v>6</v>
+      </c>
+      <c r="P46">
+        <f>COUNT(P29:P44)</f>
+        <v>16</v>
+      </c>
+      <c r="S46">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>